<commit_message>
Neue Anforderungen inkl. Klärung Fragen eingearbeitet
</commit_message>
<xml_diff>
--- a/Analysephase/Anforderungen.xlsx
+++ b/Analysephase/Anforderungen.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Fallstudie\Analysephase\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Anforderungen!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A18:F24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Anforderung</t>
   </si>
@@ -129,12 +125,6 @@
     <t>Bereichsleiter darf die Aufsummierungen für KW und Jahr für den eigenen Bereich ansehen.</t>
   </si>
   <si>
-    <t>Die Fachbereichsorganisation soll für alle Arbeitsgruppen die Zusammenfassungen für KW und Jahr ansehen können.</t>
-  </si>
-  <si>
-    <t>Die Fachbereichsorganisation soll für alle Bereiche die Zusammenfassungen für KW und Jahr ansehen können.</t>
-  </si>
-  <si>
     <t>Die Fachbereichsorganisation soll Mitarbeiter löschen können.</t>
   </si>
   <si>
@@ -177,9 +167,6 @@
     <t>zusammenrechnen Kalenderjahr</t>
   </si>
   <si>
-    <t>Die Fachbereichsorganisation soll einen Mitarbeiter unter Angabe von Benutzername, Passwort, Vorname, Nachname, Rolle und Organisationseinheit anlegen können.</t>
-  </si>
-  <si>
     <t>Rolle und Organisationseinheiten müssen über Select-Felder auswählbar sein.</t>
   </si>
   <si>
@@ -187,6 +174,78 @@
   </si>
   <si>
     <t>Die Summierung von Einträgen zu einem Kalenderjahr (1.1. - 31.12.) muss automatisiert je Arbeitsgruppe und je Bereich erfolgen.</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe anlegen</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe ändern</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe löschen</t>
+  </si>
+  <si>
+    <t>Bereich anlegen</t>
+  </si>
+  <si>
+    <t>Bereich ändern</t>
+  </si>
+  <si>
+    <t>Bereich löschen</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll eine Arbeitsgruppe mit Angabe der Kurzbezeichnung, Bezeichnung und des Bereiches (Select!) anlegen können.</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll eine Arbeitsgruppe löschen können.</t>
+  </si>
+  <si>
+    <t>inaktiv setzen!</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll einen Bereich mit Angabe der Kurzbezeichnung und Bezeichnung anlegen können</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll bei einem Bereich die Kurzbezeichnung, Bezeichnung und den Leiter ändern können.</t>
+  </si>
+  <si>
+    <t>Leiter aus Select-Feld ziehen!</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorgansiation soll einen Bereich löschen können.</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll bei einer Arbeitsgruppe die Zuordnung zum Bereich, die Kurzbezeichnung, die Bezeichnung und den Arbeitsgrupppenleiter ändern können.</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation und der Zentralbereichsleiter sollen für alle Bereiche die Zusammenfassungen für KW und Jahr ansehen können.</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation und der Zentralbereichsleiter sollen für alle Arbeitsgruppen die Zusammenfassungen für KW und Jahr ansehen können.</t>
+  </si>
+  <si>
+    <t>Zentralbereichsleiter</t>
+  </si>
+  <si>
+    <t>Chef der Bereiche und der Fachbereichsorganisation</t>
+  </si>
+  <si>
+    <t>Radio-Buttons</t>
+  </si>
+  <si>
+    <t>Passwort vergessen</t>
+  </si>
+  <si>
+    <t>Bei vergessenem Passwort soll eine Hotline angegeben werden.</t>
+  </si>
+  <si>
+    <t>Passwort ändern</t>
+  </si>
+  <si>
+    <t>Jeder User soll das eigene Passwort ändern können.</t>
+  </si>
+  <si>
+    <t>Die Fachbereichsorganisation soll einen Mitarbeiter unter Angabe von Benutzername, Passwort (generieren?), Vorname, Nachname, Rolle und Organisationseinheit anlegen können.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -581,6 +640,9 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
@@ -618,7 +680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="42.75">
+    <row r="8" spans="1:5" ht="57">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -626,10 +688,10 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42.75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -637,7 +699,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.5">
@@ -684,10 +746,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5">
@@ -698,7 +760,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42.75">
@@ -709,7 +771,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="42.75">
@@ -717,24 +779,27 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="42.75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="42.75">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="42.75">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="42.75">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
@@ -742,43 +807,143 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="42.75">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="57">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
       <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="28.5">
+      <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="42.75">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="42.75">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="28.5">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="28.5">
+      <c r="A25" s="1">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1">
+      <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.5">
-      <c r="B21" s="1" t="s">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="28.5">
+      <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="1" t="s">
+    <row r="31" spans="1:5" s="1" customFormat="1">
+      <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="1" t="s">
+    <row r="32" spans="1:5" s="1" customFormat="1">
+      <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="1" t="s">
+    <row r="33" spans="1:5" s="1" customFormat="1">
+      <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -791,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -805,42 +970,50 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Änderung UseCases und Anpassen Anforderungen
</commit_message>
<xml_diff>
--- a/Analysephase/Anforderungen.xlsx
+++ b/Analysephase/Anforderungen.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\git\Fallstudie\Analysephase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6450"/>
   </bookViews>
@@ -14,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Anforderungen!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A18:F24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,18 +183,12 @@
     <t>Arbeitsgruppe anlegen</t>
   </si>
   <si>
-    <t>Arbeitsgruppe ändern</t>
-  </si>
-  <si>
     <t>Arbeitsgruppe löschen</t>
   </si>
   <si>
     <t>Bereich anlegen</t>
   </si>
   <si>
-    <t>Bereich ändern</t>
-  </si>
-  <si>
     <t>Bereich löschen</t>
   </si>
   <si>
@@ -246,13 +244,19 @@
   </si>
   <si>
     <t>Die Fachbereichsorganisation soll einen Mitarbeiter unter Angabe von Benutzername, Passwort (generieren?), Vorname, Nachname, Rolle und Organisationseinheit anlegen können.</t>
+  </si>
+  <si>
+    <t>Arbeitsgruppe bearbeiten</t>
+  </si>
+  <si>
+    <t>Bereich bearbeiten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,21 +575,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B27" sqref="A27:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -616,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -630,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -641,13 +645,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -658,7 +662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -669,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -680,7 +684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="57">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -688,10 +692,10 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -699,10 +703,10 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -713,7 +717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.5">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -724,7 +728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -738,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -746,13 +750,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.5">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -763,7 +767,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42.75">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -774,7 +778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42.75">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -785,7 +789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="42.75">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -796,7 +800,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="42.75">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -807,7 +811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="42.75">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -815,99 +819,96 @@
         <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="57">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" ht="28.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" ht="42.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" ht="42.75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" ht="28.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="28.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="1" customFormat="1">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="29" spans="1:5" s="1" customFormat="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
@@ -915,7 +916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="28.5">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
@@ -923,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="1" customFormat="1">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
@@ -931,7 +932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
@@ -939,7 +940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
@@ -962,13 +963,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -976,7 +977,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -984,7 +985,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -992,7 +993,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1008,12 +1009,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>